<commit_message>
Enhance invoice data capture to include all form fields
Add comprehensive field extraction using JavaScript page.evaluate() to capture
all visible data from the invoice form including client details, bank account
information, and transaction details. The report now displays 22 fields instead
of the previous minimal set.

🤖 Generated with [Claude Code](https://claude.com/claude-code)

Co-Authored-By: Claude Opus 4.5 <noreply@anthropic.com>
</commit_message>
<xml_diff>
--- a/Testcase/OB_Automation.xlsx
+++ b/Testcase/OB_Automation.xlsx
@@ -8,21 +8,20 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Vishesh\OmneyBusiness\Testcase\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:2001_{E11561F6-4921-4AC1-80EA-07402A495636}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6B023902-E731-4C2A-A22D-418BE9D5012D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="20370" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Testcase" sheetId="1" r:id="rId1"/>
     <sheet name="Invoice" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="0"/>
-  <fileRecoveryPr repairLoad="1"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="93" uniqueCount="90">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="98" uniqueCount="94">
   <si>
     <t>TC_ID</t>
   </si>
@@ -46,12 +45,6 @@
   </si>
   <si>
     <t>To check if URL is working</t>
-  </si>
-  <si>
-    <t>1. Navidate to URL</t>
-  </si>
-  <si>
-    <t>Url should be working</t>
   </si>
   <si>
     <t>High</t>
@@ -122,37 +115,19 @@
     <t xml:space="preserve">User Pays invoice without Completing profile- P &amp; B </t>
   </si>
   <si>
-    <t>To complete profile with Individual Acocunt</t>
-  </si>
-  <si>
     <t>To Raise an Invoice as Individual</t>
   </si>
   <si>
     <t>To Raise an Invoice as Business</t>
   </si>
   <si>
-    <t>To Pay Invoice as Individiual</t>
-  </si>
-  <si>
     <t>To Pay Invoice as Business</t>
   </si>
   <si>
-    <t>To Add a Client as Indiviudal</t>
-  </si>
-  <si>
     <t>To Add a Client as Business</t>
   </si>
   <si>
-    <t>To Add a Vendor as Indiviudal</t>
-  </si>
-  <si>
     <t>To Add a Vendor as Business</t>
-  </si>
-  <si>
-    <t>To Raise Invoce and Check for Pending Receivables</t>
-  </si>
-  <si>
-    <t>To Raise Invoce and Check for Pending Payables</t>
   </si>
   <si>
     <t>To check Pending Invoice Raised</t>
@@ -302,6 +277,46 @@
   </si>
   <si>
     <t xml:space="preserve">A pop up will display with Request ID </t>
+  </si>
+  <si>
+    <t>Raise invoice but client is not registered</t>
+  </si>
+  <si>
+    <t>Send Reminder</t>
+  </si>
+  <si>
+    <t>To Add a Vendor as Individual</t>
+  </si>
+  <si>
+    <t>To Add a Client as Individual</t>
+  </si>
+  <si>
+    <t>To Pay Invoice as Individual</t>
+  </si>
+  <si>
+    <t>To Raise Invoice and Check for Pending Payables</t>
+  </si>
+  <si>
+    <t>1. Navigate to URL</t>
+  </si>
+  <si>
+    <t>URL should be working</t>
+  </si>
+  <si>
+    <t>To complete profile with Individual Account</t>
+  </si>
+  <si>
+    <t>To check for Pending Receivables</t>
+  </si>
+  <si>
+    <t>1. This is continuation of TC_03
+2. After Close button is clicked, check Under Pending Receivables
+3. Look for same Request ID which was saved during TC_03
+4. Click on the Eye icon on the right end side of the same row (a view page will Open)
+5. Verify the data in the view page with the Transaction data stored in TC_03</t>
+  </si>
+  <si>
+    <t>All data in view page should be same as per the Create Invoice page</t>
   </si>
 </sst>
 </file>
@@ -683,10 +698,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:F31"/>
+  <dimension ref="A1:F33"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C6" sqref="C6"/>
+    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="C8" sqref="C8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -727,77 +742,81 @@
         <v>7</v>
       </c>
       <c r="C2" s="2" t="s">
+        <v>88</v>
+      </c>
+      <c r="D2" t="s">
+        <v>25</v>
+      </c>
+      <c r="E2" s="2" t="s">
+        <v>89</v>
+      </c>
+      <c r="F2" s="2" t="s">
         <v>8</v>
-      </c>
-      <c r="D2" t="s">
-        <v>27</v>
-      </c>
-      <c r="E2" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="F2" s="2" t="s">
-        <v>10</v>
       </c>
     </row>
     <row r="3" spans="1:6" ht="60" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="B3" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="C3" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="B3" s="2" t="s">
+      <c r="D3" s="2" t="s">
+        <v>59</v>
+      </c>
+      <c r="E3" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="C3" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="D3" s="2" t="s">
-        <v>67</v>
-      </c>
-      <c r="E3" s="2" t="s">
-        <v>14</v>
-      </c>
       <c r="F3" s="2" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
     </row>
     <row r="4" spans="1:6" ht="120" x14ac:dyDescent="0.25">
       <c r="A4" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="B4" s="2" t="s">
+        <v>78</v>
+      </c>
+      <c r="C4" s="2" t="s">
+        <v>79</v>
+      </c>
+      <c r="D4" s="2" t="s">
+        <v>80</v>
+      </c>
+      <c r="E4" s="2" t="s">
+        <v>81</v>
+      </c>
+      <c r="F4" s="2" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" ht="120" x14ac:dyDescent="0.25">
+      <c r="A5" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="B5" s="2" t="s">
+        <v>91</v>
+      </c>
+      <c r="C5" s="2" t="s">
+        <v>92</v>
+      </c>
+      <c r="D5" s="2"/>
+      <c r="E5" s="2" t="s">
+        <v>93</v>
+      </c>
+      <c r="F5" s="2" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A6" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="B4" s="2" t="s">
-        <v>86</v>
-      </c>
-      <c r="C4" s="2" t="s">
-        <v>87</v>
-      </c>
-      <c r="D4" s="2" t="s">
-        <v>88</v>
-      </c>
-      <c r="E4" s="2" t="s">
-        <v>89</v>
-      </c>
-      <c r="F4" s="2" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A5" s="2" t="s">
-        <v>16</v>
-      </c>
-      <c r="B5" s="2" t="s">
-        <v>28</v>
-      </c>
-      <c r="C5" s="2"/>
-      <c r="D5" s="2"/>
-      <c r="E5" s="2"/>
-      <c r="F5" s="2"/>
-    </row>
-    <row r="6" spans="1:6" ht="30" x14ac:dyDescent="0.25">
-      <c r="A6" s="2" t="s">
-        <v>17</v>
-      </c>
-      <c r="B6" s="2" t="s">
-        <v>32</v>
-      </c>
+      <c r="B6" s="2"/>
       <c r="C6" s="2"/>
       <c r="D6" s="2"/>
       <c r="E6" s="2"/>
@@ -805,10 +824,10 @@
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A7" s="2" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="B7" s="2" t="s">
-        <v>29</v>
+        <v>26</v>
       </c>
       <c r="C7" s="2"/>
       <c r="D7" s="2"/>
@@ -817,10 +836,10 @@
     </row>
     <row r="8" spans="1:6" ht="30" x14ac:dyDescent="0.25">
       <c r="A8" s="2" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="B8" s="2" t="s">
-        <v>32</v>
+        <v>90</v>
       </c>
       <c r="C8" s="2"/>
       <c r="D8" s="2"/>
@@ -829,22 +848,22 @@
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A9" s="2" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="B9" s="2" t="s">
-        <v>39</v>
+        <v>27</v>
       </c>
       <c r="C9" s="2"/>
       <c r="D9" s="2"/>
       <c r="E9" s="2"/>
       <c r="F9" s="2"/>
     </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:6" ht="30" x14ac:dyDescent="0.25">
       <c r="A10" s="2" t="s">
-        <v>21</v>
-      </c>
-      <c r="B10" t="s">
-        <v>40</v>
+        <v>19</v>
+      </c>
+      <c r="B10" s="2" t="s">
+        <v>90</v>
       </c>
       <c r="D10" s="2"/>
       <c r="E10" s="2"/>
@@ -852,10 +871,10 @@
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A11" s="2" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="B11" s="2" t="s">
-        <v>37</v>
+        <v>84</v>
       </c>
       <c r="D11" s="2"/>
       <c r="E11" s="2"/>
@@ -863,10 +882,10 @@
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A12" s="2" t="s">
-        <v>23</v>
-      </c>
-      <c r="B12" s="2" t="s">
-        <v>38</v>
+        <v>21</v>
+      </c>
+      <c r="B12" t="s">
+        <v>34</v>
       </c>
       <c r="D12" s="2"/>
       <c r="E12" s="2"/>
@@ -874,10 +893,10 @@
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A13" s="2" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="B13" s="2" t="s">
-        <v>33</v>
+        <v>85</v>
       </c>
       <c r="C13" s="2"/>
       <c r="D13" s="2"/>
@@ -886,10 +905,10 @@
     </row>
     <row r="14" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A14" s="2" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="B14" s="2" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="C14" s="2"/>
       <c r="D14" s="2"/>
@@ -898,10 +917,10 @@
     </row>
     <row r="15" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A15" s="2" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="B15" s="2" t="s">
-        <v>35</v>
+        <v>30</v>
       </c>
       <c r="C15" s="2"/>
       <c r="D15" s="2"/>
@@ -910,74 +929,72 @@
     </row>
     <row r="16" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A16" s="2" t="s">
-        <v>52</v>
+        <v>44</v>
       </c>
       <c r="B16" s="2" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="17" spans="1:3" ht="30" x14ac:dyDescent="0.25">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A17" s="2" t="s">
-        <v>53</v>
+        <v>45</v>
       </c>
       <c r="B17" s="2" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="18" spans="1:3" ht="30" x14ac:dyDescent="0.25">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A18" s="2" t="s">
-        <v>54</v>
+        <v>46</v>
       </c>
       <c r="B18" s="2" t="s">
-        <v>42</v>
+        <v>32</v>
       </c>
     </row>
     <row r="19" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A19" s="2" t="s">
-        <v>55</v>
-      </c>
-      <c r="B19" s="2" t="s">
+        <v>47</v>
+      </c>
+      <c r="B19" s="2"/>
+    </row>
+    <row r="20" spans="1:3" ht="30" x14ac:dyDescent="0.25">
+      <c r="A20" s="2" t="s">
         <v>48</v>
       </c>
-    </row>
-    <row r="20" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A20" s="2" t="s">
-        <v>56</v>
-      </c>
       <c r="B20" s="2" t="s">
-        <v>49</v>
+        <v>87</v>
       </c>
       <c r="C20" t="s">
-        <v>66</v>
+        <v>58</v>
       </c>
     </row>
     <row r="21" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A21" s="2" t="s">
-        <v>57</v>
+        <v>49</v>
       </c>
       <c r="B21" s="2" t="s">
-        <v>50</v>
+        <v>40</v>
       </c>
     </row>
     <row r="22" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A22" s="2" t="s">
-        <v>58</v>
+        <v>50</v>
       </c>
       <c r="B22" s="2" t="s">
-        <v>51</v>
+        <v>41</v>
       </c>
     </row>
     <row r="23" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A23" s="2" t="s">
-        <v>59</v>
+        <v>51</v>
       </c>
       <c r="B23" s="2" t="s">
-        <v>47</v>
+        <v>42</v>
       </c>
     </row>
     <row r="24" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A24" s="2" t="s">
-        <v>60</v>
+        <v>52</v>
       </c>
       <c r="B24" s="2" t="s">
         <v>43</v>
@@ -985,46 +1002,63 @@
     </row>
     <row r="25" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A25" s="2" t="s">
-        <v>61</v>
+        <v>53</v>
       </c>
       <c r="B25" s="2" t="s">
-        <v>44</v>
+        <v>39</v>
       </c>
     </row>
     <row r="26" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A26" s="2" t="s">
-        <v>62</v>
+        <v>54</v>
       </c>
       <c r="B26" s="2" t="s">
-        <v>45</v>
+        <v>35</v>
       </c>
     </row>
     <row r="27" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A27" s="2" t="s">
-        <v>63</v>
+        <v>55</v>
       </c>
       <c r="B27" s="2" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="28" spans="1:3" ht="30" x14ac:dyDescent="0.25">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="28" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A28" s="2" t="s">
-        <v>64</v>
+        <v>56</v>
       </c>
       <c r="B28" s="2" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="29" spans="1:3" ht="30" x14ac:dyDescent="0.25">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="29" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A29" s="2" t="s">
-        <v>65</v>
+        <v>57</v>
       </c>
       <c r="B29" s="2" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="31" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="B31" s="2"/>
+        <v>38</v>
+      </c>
+    </row>
+    <row r="30" spans="1:3" ht="30" x14ac:dyDescent="0.25">
+      <c r="B30" s="2" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="31" spans="1:3" ht="30" x14ac:dyDescent="0.25">
+      <c r="B31" s="2" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="32" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B32" s="2" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="33" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B33" s="2" t="s">
+        <v>83</v>
+      </c>
     </row>
   </sheetData>
   <phoneticPr fontId="3" type="noConversion"/>
@@ -1050,34 +1084,34 @@
   <sheetData>
     <row r="1" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
+        <v>60</v>
+      </c>
+      <c r="B1" t="s">
+        <v>61</v>
+      </c>
+      <c r="C1" t="s">
+        <v>63</v>
+      </c>
+      <c r="D1" t="s">
+        <v>65</v>
+      </c>
+      <c r="E1" t="s">
         <v>68</v>
       </c>
-      <c r="B1" t="s">
+      <c r="F1" t="s">
         <v>69</v>
       </c>
-      <c r="C1" t="s">
+      <c r="G1" t="s">
         <v>71</v>
       </c>
-      <c r="D1" t="s">
+      <c r="H1" t="s">
         <v>73</v>
       </c>
-      <c r="E1" t="s">
+      <c r="I1" t="s">
+        <v>74</v>
+      </c>
+      <c r="J1" t="s">
         <v>76</v>
-      </c>
-      <c r="F1" t="s">
-        <v>77</v>
-      </c>
-      <c r="G1" t="s">
-        <v>79</v>
-      </c>
-      <c r="H1" t="s">
-        <v>81</v>
-      </c>
-      <c r="I1" t="s">
-        <v>82</v>
-      </c>
-      <c r="J1" t="s">
-        <v>84</v>
       </c>
     </row>
     <row r="2" spans="1:10" x14ac:dyDescent="0.25">
@@ -1085,31 +1119,31 @@
         <v>1</v>
       </c>
       <c r="B2" t="s">
+        <v>62</v>
+      </c>
+      <c r="C2" t="s">
+        <v>64</v>
+      </c>
+      <c r="D2" t="s">
+        <v>66</v>
+      </c>
+      <c r="E2" t="s">
+        <v>67</v>
+      </c>
+      <c r="F2" t="s">
         <v>70</v>
       </c>
-      <c r="C2" t="s">
+      <c r="G2" t="s">
         <v>72</v>
-      </c>
-      <c r="D2" t="s">
-        <v>74</v>
-      </c>
-      <c r="E2" t="s">
-        <v>75</v>
-      </c>
-      <c r="F2" t="s">
-        <v>78</v>
-      </c>
-      <c r="G2" t="s">
-        <v>80</v>
       </c>
       <c r="H2">
         <v>5000</v>
       </c>
       <c r="I2" t="s">
-        <v>83</v>
+        <v>75</v>
       </c>
       <c r="J2" t="s">
-        <v>85</v>
+        <v>77</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Add TC_04 - Verify Pending Receivables test case
- Integrate TC_04 into main automation script (omney_business_automation.py)
- Add standalone TC_04 script for independent execution
- TC_04 finds invoice in Pending Receivables and verifies data against TC_03
- Add verification results table to HTML report with Expected vs Actual comparison
- Add observations section highlighting mismatched/missing fields

🤖 Generated with [Claude Code](https://claude.com/claude-code)

Co-Authored-By: Claude Opus 4.5 <noreply@anthropic.com>
</commit_message>
<xml_diff>
--- a/Testcase/OB_Automation.xlsx
+++ b/Testcase/OB_Automation.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Vishesh\OmneyBusiness\Testcase\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6B023902-E731-4C2A-A22D-418BE9D5012D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{447BCCDC-CCAB-48E6-9A77-FE22A81BD131}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -309,14 +309,14 @@
     <t>To check for Pending Receivables</t>
   </si>
   <si>
+    <t>All data in view page should be same as per the Create Invoice page</t>
+  </si>
+  <si>
     <t>1. This is continuation of TC_03
 2. After Close button is clicked, check Under Pending Receivables
-3. Look for same Request ID which was saved during TC_03
+3. Look for same Invoice Number which was created and saved during TC_03
 4. Click on the Eye icon on the right end side of the same row (a view page will Open)
 5. Verify the data in the view page with the Transaction data stored in TC_03</t>
-  </si>
-  <si>
-    <t>All data in view page should be same as per the Create Invoice page</t>
   </si>
 </sst>
 </file>
@@ -700,8 +700,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:F33"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="C8" sqref="C8"/>
+    <sheetView tabSelected="1" topLeftCell="A3" workbookViewId="0">
+      <selection activeCell="C5" sqref="C5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -794,7 +794,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="5" spans="1:6" ht="120" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:6" ht="135" x14ac:dyDescent="0.25">
       <c r="A5" s="2" t="s">
         <v>14</v>
       </c>
@@ -802,11 +802,11 @@
         <v>91</v>
       </c>
       <c r="C5" s="2" t="s">
-        <v>92</v>
+        <v>93</v>
       </c>
       <c r="D5" s="2"/>
       <c r="E5" s="2" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="F5" s="2" t="s">
         <v>8</v>

</xml_diff>